<commit_message>
added the batchid for current expense table
</commit_message>
<xml_diff>
--- a/data/monthly_exp.xlsx
+++ b/data/monthly_exp.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="734" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="734" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Estimated" sheetId="1" r:id="rId1"/>
@@ -343,10 +343,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1475,19 +1475,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L13" s="15" t="s">
+      <c r="L13" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="15"/>
-      <c r="S13" s="15"/>
-      <c r="T13" s="15"/>
-      <c r="U13" s="15"/>
-      <c r="V13" s="15"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="16"/>
+      <c r="S13" s="16"/>
+      <c r="T13" s="16"/>
+      <c r="U13" s="16"/>
+      <c r="V13" s="16"/>
     </row>
     <row r="14" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -1642,7 +1642,7 @@
       <c r="M19" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="N19" s="16" t="s">
+      <c r="N19" s="15" t="s">
         <v>55</v>
       </c>
       <c r="O19" s="4"/>
@@ -1661,7 +1661,7 @@
       <c r="M20" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="N20" s="16" t="s">
+      <c r="N20" s="15" t="s">
         <v>55</v>
       </c>
       <c r="O20" s="4"/>
@@ -1680,7 +1680,7 @@
       <c r="M21" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="N21" s="16" t="s">
+      <c r="N21" s="15" t="s">
         <v>55</v>
       </c>
       <c r="O21" s="4"/>
@@ -1699,7 +1699,7 @@
       <c r="M22" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="N22" s="16" t="s">
+      <c r="N22" s="15" t="s">
         <v>55</v>
       </c>
       <c r="O22" s="4"/>
@@ -1718,7 +1718,7 @@
       <c r="M23" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="N23" s="16" t="s">
+      <c r="N23" s="15" t="s">
         <v>55</v>
       </c>
       <c r="O23" s="4"/>
@@ -1994,7 +1994,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2020,6 +2020,9 @@
       <c r="A2" t="s">
         <v>11</v>
       </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
       <c r="C2">
         <v>3000</v>
       </c>
@@ -2043,6 +2046,9 @@
       <c r="D3">
         <v>1360</v>
       </c>
+      <c r="E3">
+        <v>2869</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -2056,105 +2062,162 @@
       </c>
       <c r="D4">
         <v>230</v>
+      </c>
+      <c r="E4">
+        <v>2869</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
       <c r="C5">
         <v>200</v>
       </c>
       <c r="D5">
         <v>0</v>
+      </c>
+      <c r="E5">
+        <v>2869</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
       <c r="C6">
         <v>129</v>
       </c>
       <c r="D6">
         <v>0</v>
+      </c>
+      <c r="E6">
+        <v>2869</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
       <c r="C7">
         <v>145</v>
       </c>
       <c r="D7">
         <v>0</v>
+      </c>
+      <c r="E7">
+        <v>2869</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
       <c r="C8">
         <v>950</v>
       </c>
       <c r="D8">
         <v>0</v>
+      </c>
+      <c r="E8">
+        <v>2869</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
       <c r="C9">
         <v>1400</v>
       </c>
       <c r="D9">
         <v>0</v>
+      </c>
+      <c r="E9">
+        <v>2869</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
       <c r="C10">
         <v>1400</v>
       </c>
       <c r="D10">
         <v>0</v>
+      </c>
+      <c r="E10">
+        <v>2869</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
       <c r="C11">
         <v>110</v>
       </c>
       <c r="D11">
         <v>0</v>
+      </c>
+      <c r="E11">
+        <v>2869</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
       <c r="C12">
         <v>500</v>
       </c>
       <c r="D12">
         <v>0</v>
+      </c>
+      <c r="E12">
+        <v>2869</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
       <c r="C13">
         <v>500</v>
       </c>
       <c r="D13">
         <v>0</v>
+      </c>
+      <c r="E13">
+        <v>2869</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2170,16 +2233,25 @@
       <c r="D14">
         <v>400</v>
       </c>
+      <c r="E14">
+        <v>2869</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
       <c r="C15">
         <v>900</v>
       </c>
       <c r="D15">
         <v>0</v>
+      </c>
+      <c r="E15">
+        <v>2869</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2195,8 +2267,11 @@
       <c r="D16">
         <v>846</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>2869</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -2209,16 +2284,25 @@
       <c r="D17">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>2869</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
       <c r="C18">
         <v>1000</v>
       </c>
       <c r="D18">
         <v>1000</v>
+      </c>
+      <c r="E18">
+        <v>2869</v>
       </c>
     </row>
   </sheetData>
@@ -2273,8 +2357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2326,6 +2410,9 @@
       <c r="D3">
         <v>5440</v>
       </c>
+      <c r="E3">
+        <v>23784</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -2339,6 +2426,9 @@
       </c>
       <c r="D4">
         <v>1500</v>
+      </c>
+      <c r="E4">
+        <v>23784</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2354,6 +2444,9 @@
       <c r="D5">
         <v>200</v>
       </c>
+      <c r="E5">
+        <v>23784</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -2368,6 +2461,9 @@
       <c r="D6">
         <v>129</v>
       </c>
+      <c r="E6">
+        <v>23784</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -2382,6 +2478,9 @@
       <c r="D7">
         <v>145</v>
       </c>
+      <c r="E7">
+        <v>23784</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -2396,6 +2495,9 @@
       <c r="D8">
         <v>950</v>
       </c>
+      <c r="E8">
+        <v>23784</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -2410,6 +2512,9 @@
       <c r="D9">
         <v>1400</v>
       </c>
+      <c r="E9">
+        <v>23784</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -2424,6 +2529,9 @@
       <c r="D10">
         <v>1400</v>
       </c>
+      <c r="E10">
+        <v>23784</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -2438,6 +2546,9 @@
       <c r="D11">
         <v>1320</v>
       </c>
+      <c r="E11">
+        <v>23784</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -2452,6 +2563,9 @@
       <c r="D12">
         <v>2000</v>
       </c>
+      <c r="E12">
+        <v>23784</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -2466,6 +2580,9 @@
       <c r="D13">
         <v>1000</v>
       </c>
+      <c r="E13">
+        <v>23784</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -2480,6 +2597,9 @@
       <c r="D14">
         <v>900</v>
       </c>
+      <c r="E14">
+        <v>23784</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -2494,6 +2614,9 @@
       <c r="D15">
         <v>400</v>
       </c>
+      <c r="E15">
+        <v>23784</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -2508,8 +2631,11 @@
       <c r="D16">
         <v>3000</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>23784</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -2521,6 +2647,9 @@
       </c>
       <c r="D17">
         <v>1000</v>
+      </c>
+      <c r="E17">
+        <v>23784</v>
       </c>
     </row>
   </sheetData>
@@ -2532,7 +2661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added the actual and current expense table in the ui
</commit_message>
<xml_diff>
--- a/data/monthly_exp.xlsx
+++ b/data/monthly_exp.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="734" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="734" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Estimated" sheetId="1" r:id="rId1"/>
@@ -944,6 +944,9 @@
       <c r="A2" t="s">
         <v>11</v>
       </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
       <c r="C2">
         <v>3000</v>
       </c>
@@ -953,18 +956,18 @@
       </c>
       <c r="E2">
         <f>SUM(D2:D17)</f>
-        <v>2869</v>
+        <v>7364</v>
       </c>
       <c r="G2">
-        <f>E2+17557</f>
-        <v>20426</v>
+        <f>21000</f>
+        <v>21000</v>
       </c>
       <c r="H2">
-        <f>G2-E2</f>
-        <v>17557</v>
+        <f>G2-E2-H5</f>
+        <v>12636</v>
       </c>
       <c r="I2">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L2" t="s">
         <v>16</v>
@@ -1017,6 +1020,9 @@
         <f t="shared" si="0"/>
         <v>1360</v>
       </c>
+      <c r="E3">
+        <v>7080</v>
+      </c>
       <c r="L3" t="s">
         <v>0</v>
       </c>
@@ -1061,14 +1067,17 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="C4">
         <v>10</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>230</v>
+        <v>510</v>
+      </c>
+      <c r="E4">
+        <v>7080</v>
       </c>
       <c r="L4" t="s">
         <v>1</v>
@@ -1113,12 +1122,18 @@
       <c r="A5" t="s">
         <v>2</v>
       </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
       <c r="C5">
         <v>200</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>200</v>
+      </c>
+      <c r="E5">
+        <v>7080</v>
       </c>
       <c r="G5" t="s">
         <v>25</v>
@@ -1170,12 +1185,18 @@
       <c r="A6" t="s">
         <v>3</v>
       </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
       <c r="C6">
         <v>129</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+      <c r="E6">
+        <v>7080</v>
       </c>
       <c r="L6" t="s">
         <v>7</v>
@@ -1217,12 +1238,18 @@
       <c r="A7" t="s">
         <v>4</v>
       </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
       <c r="C7">
         <v>145</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+      <c r="E7">
+        <v>7080</v>
       </c>
       <c r="L7" t="s">
         <v>8</v>
@@ -1264,12 +1291,18 @@
       <c r="A8" t="s">
         <v>5</v>
       </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
       <c r="C8">
         <v>950</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+      <c r="E8">
+        <v>7080</v>
       </c>
       <c r="L8" t="s">
         <v>9</v>
@@ -1311,12 +1344,18 @@
       <c r="A9" t="s">
         <v>6</v>
       </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
       <c r="C9">
-        <v>1400</v>
+        <v>790</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C9</f>
+        <v>790</v>
+      </c>
+      <c r="E9">
+        <v>7080</v>
       </c>
       <c r="L9" t="s">
         <v>10</v>
@@ -1358,12 +1397,18 @@
       <c r="A10" t="s">
         <v>7</v>
       </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
       <c r="C10">
-        <v>1400</v>
+        <v>1160</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C10</f>
+        <v>1160</v>
+      </c>
+      <c r="E10">
+        <v>7080</v>
       </c>
       <c r="L10" t="s">
         <v>13</v>
@@ -1386,11 +1431,11 @@
       </c>
       <c r="R10">
         <f>C16</f>
-        <v>846</v>
+        <v>1849</v>
       </c>
       <c r="S10" s="1">
         <f t="shared" si="2"/>
-        <v>846</v>
+        <v>1849</v>
       </c>
       <c r="T10" t="s">
         <v>13</v>
@@ -1407,12 +1452,18 @@
       <c r="A11" t="s">
         <v>8</v>
       </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
       <c r="C11">
         <v>110</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+      <c r="E11">
+        <v>7080</v>
       </c>
       <c r="L11" t="s">
         <v>14</v>
@@ -1435,11 +1486,11 @@
       </c>
       <c r="R11">
         <f>C17</f>
-        <v>33</v>
+        <v>125</v>
       </c>
       <c r="S11" s="1">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>125</v>
       </c>
       <c r="T11" t="s">
         <v>14</v>
@@ -1456,24 +1507,36 @@
       <c r="A12" t="s">
         <v>9</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C12</f>
+        <v>700</v>
+      </c>
+      <c r="E12">
+        <v>7080</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
       <c r="C13">
-        <v>500</v>
+        <v>270</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C13</f>
+        <v>270</v>
+      </c>
+      <c r="E13">
+        <v>7080</v>
       </c>
       <c r="L13" s="16" t="s">
         <v>29</v>
@@ -1502,6 +1565,9 @@
       <c r="D14">
         <f>C14*B14</f>
         <v>400</v>
+      </c>
+      <c r="E14">
+        <v>7080</v>
       </c>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
@@ -1519,12 +1585,18 @@
       <c r="A15" t="s">
         <v>12</v>
       </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
       <c r="C15">
         <v>900</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+      <c r="E15">
+        <v>7080</v>
       </c>
       <c r="L15" s="5" t="s">
         <v>16</v>
@@ -1550,11 +1622,15 @@
         <v>1</v>
       </c>
       <c r="C16">
-        <v>846</v>
+        <f>1560+171+82+36</f>
+        <v>1849</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>846</v>
+        <v>1849</v>
+      </c>
+      <c r="E16">
+        <v>7080</v>
       </c>
       <c r="L16" s="9" t="s">
         <v>0</v>
@@ -1582,11 +1658,15 @@
         <v>1</v>
       </c>
       <c r="C17">
-        <v>33</v>
+        <f>37+8+80</f>
+        <v>125</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>125</v>
+      </c>
+      <c r="E17">
+        <v>7080</v>
       </c>
       <c r="L17" s="9" t="s">
         <v>1</v>
@@ -1610,12 +1690,18 @@
       <c r="A18" t="s">
         <v>20</v>
       </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
       <c r="C18">
         <v>1000</v>
       </c>
       <c r="D18">
         <f>C18</f>
         <v>1000</v>
+      </c>
+      <c r="E18">
+        <v>7080</v>
       </c>
       <c r="L18" s="9" t="s">
         <v>6</v>
@@ -1994,7 +2080,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2030,7 +2116,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>2869</v>
+        <v>7364</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2047,7 +2133,7 @@
         <v>1360</v>
       </c>
       <c r="E3">
-        <v>2869</v>
+        <v>7080</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2055,16 +2141,16 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="C4">
         <v>10</v>
       </c>
       <c r="D4">
-        <v>230</v>
+        <v>510</v>
       </c>
       <c r="E4">
-        <v>2869</v>
+        <v>7080</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2072,16 +2158,16 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>200</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E5">
-        <v>2869</v>
+        <v>7080</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2098,7 +2184,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>2869</v>
+        <v>7080</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2115,7 +2201,7 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>2869</v>
+        <v>7080</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2132,7 +2218,7 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>2869</v>
+        <v>7080</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2140,16 +2226,16 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>1400</v>
+        <v>790</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>790</v>
       </c>
       <c r="E9">
-        <v>2869</v>
+        <v>7080</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2157,16 +2243,16 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>1400</v>
+        <v>1160</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1160</v>
       </c>
       <c r="E10">
-        <v>2869</v>
+        <v>7080</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2183,7 +2269,7 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>2869</v>
+        <v>7080</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2191,16 +2277,16 @@
         <v>9</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="E12">
-        <v>2869</v>
+        <v>7080</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2208,16 +2294,16 @@
         <v>10</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>500</v>
+        <v>270</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>270</v>
       </c>
       <c r="E13">
-        <v>2869</v>
+        <v>7080</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2234,7 +2320,7 @@
         <v>400</v>
       </c>
       <c r="E14">
-        <v>2869</v>
+        <v>7080</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2251,7 +2337,7 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>2869</v>
+        <v>7080</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2262,13 +2348,13 @@
         <v>1</v>
       </c>
       <c r="C16">
-        <v>846</v>
+        <v>1849</v>
       </c>
       <c r="D16">
-        <v>846</v>
+        <v>1849</v>
       </c>
       <c r="E16">
-        <v>2869</v>
+        <v>7080</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2279,13 +2365,13 @@
         <v>1</v>
       </c>
       <c r="C17">
-        <v>33</v>
+        <v>125</v>
       </c>
       <c r="D17">
-        <v>33</v>
+        <v>125</v>
       </c>
       <c r="E17">
-        <v>2869</v>
+        <v>7080</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2302,7 +2388,7 @@
         <v>1000</v>
       </c>
       <c r="E18">
-        <v>2869</v>
+        <v>7080</v>
       </c>
     </row>
   </sheetData>
@@ -2314,8 +2400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2336,13 +2422,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>20426</v>
+        <v>21000</v>
       </c>
       <c r="B2">
-        <v>17557</v>
+        <v>12636</v>
       </c>
       <c r="C2">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D2">
         <v>1000</v>
@@ -2357,8 +2443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
corrected the expense rules
</commit_message>
<xml_diff>
--- a/data/monthly_exp.xlsx
+++ b/data/monthly_exp.xlsx
@@ -956,7 +956,7 @@
       </c>
       <c r="E2">
         <f>SUM(D2:D17)</f>
-        <v>7364</v>
+        <v>8774</v>
       </c>
       <c r="G2">
         <f>21000</f>
@@ -964,10 +964,10 @@
       </c>
       <c r="H2">
         <f>G2-E2-H5</f>
-        <v>12636</v>
+        <v>11226</v>
       </c>
       <c r="I2">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L2" t="s">
         <v>16</v>
@@ -1011,14 +1011,14 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>680</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>1360</v>
+        <v>2720</v>
       </c>
       <c r="E3">
         <v>7080</v>
@@ -1067,14 +1067,14 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C4">
         <v>10</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>510</v>
+        <v>560</v>
       </c>
       <c r="E4">
         <v>7080</v>
@@ -2080,7 +2080,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection sqref="A1:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2116,7 +2116,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>7364</v>
+        <v>8774</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2124,13 +2124,13 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>680</v>
       </c>
       <c r="D3">
-        <v>1360</v>
+        <v>2720</v>
       </c>
       <c r="E3">
         <v>7080</v>
@@ -2141,13 +2141,13 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C4">
         <v>10</v>
       </c>
       <c r="D4">
-        <v>510</v>
+        <v>560</v>
       </c>
       <c r="E4">
         <v>7080</v>
@@ -2401,7 +2401,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2425,10 +2425,10 @@
         <v>21000</v>
       </c>
       <c r="B2">
-        <v>12636</v>
+        <v>11226</v>
       </c>
       <c r="C2">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D2">
         <v>1000</v>

</xml_diff>

<commit_message>
database integration is completed
</commit_message>
<xml_diff>
--- a/data/monthly_exp.xlsx
+++ b/data/monthly_exp.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="734" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="734" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Estimated" sheetId="1" r:id="rId1"/>
@@ -893,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2400,7 +2400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added the updated cron_main.py after  inserting the base template functionality.
</commit_message>
<xml_diff>
--- a/data/monthly_exp.xlsx
+++ b/data/monthly_exp.xlsx
@@ -9,16 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="734" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="734" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Estimated" sheetId="1" r:id="rId1"/>
-    <sheet name="Actual" sheetId="2" r:id="rId2"/>
-    <sheet name="App_Layout" sheetId="3" r:id="rId3"/>
-    <sheet name="actual_cost_v1" sheetId="4" r:id="rId4"/>
-    <sheet name="current_total_expense_v1" sheetId="5" r:id="rId5"/>
-    <sheet name="planned_estimated_cost_v1" sheetId="7" r:id="rId6"/>
-    <sheet name="expense_growth_rate_v1" sheetId="6" r:id="rId7"/>
+    <sheet name="current_total_expense_base" sheetId="8" r:id="rId2"/>
+    <sheet name="Actual" sheetId="2" r:id="rId3"/>
+    <sheet name="App_Layout" sheetId="3" r:id="rId4"/>
+    <sheet name="actual_cost_v1" sheetId="4" r:id="rId5"/>
+    <sheet name="current_total_expense_v1" sheetId="5" r:id="rId6"/>
+    <sheet name="planned_estimated_cost_v1" sheetId="7" r:id="rId7"/>
+    <sheet name="expense_growth_rate_v1" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="58">
   <si>
     <t>rum</t>
   </si>
@@ -201,6 +202,9 @@
   </si>
   <si>
     <t>&lt;= 500/2 weeks</t>
+  </si>
+  <si>
+    <t>Cumulative_Quantity</t>
   </si>
 </sst>
 </file>
@@ -891,10 +895,385 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F4:F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>3000</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>8774</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>680</v>
+      </c>
+      <c r="D3">
+        <v>2720</v>
+      </c>
+      <c r="E3">
+        <v>7080</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>56</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>560</v>
+      </c>
+      <c r="E4">
+        <v>7080</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>200</v>
+      </c>
+      <c r="D5">
+        <v>200</v>
+      </c>
+      <c r="E5">
+        <v>7080</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>129</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>7080</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>145</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>7080</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>950</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>7080</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>790</v>
+      </c>
+      <c r="D9">
+        <v>790</v>
+      </c>
+      <c r="E9">
+        <v>7080</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1160</v>
+      </c>
+      <c r="D10">
+        <v>1160</v>
+      </c>
+      <c r="E10">
+        <v>7080</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>110</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>7080</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>700</v>
+      </c>
+      <c r="D12">
+        <v>700</v>
+      </c>
+      <c r="E12">
+        <v>7080</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>270</v>
+      </c>
+      <c r="D13">
+        <v>270</v>
+      </c>
+      <c r="E13">
+        <v>7080</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>400</v>
+      </c>
+      <c r="D14">
+        <v>400</v>
+      </c>
+      <c r="E14">
+        <v>7080</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>900</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>7080</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1849</v>
+      </c>
+      <c r="D16">
+        <v>1849</v>
+      </c>
+      <c r="E16">
+        <v>7080</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>125</v>
+      </c>
+      <c r="D17">
+        <v>125</v>
+      </c>
+      <c r="E17">
+        <v>7080</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>1000</v>
+      </c>
+      <c r="D18">
+        <v>1000</v>
+      </c>
+      <c r="E18">
+        <v>7080</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1841,7 +2220,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
@@ -2075,7 +2454,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
@@ -2396,7 +2775,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2439,12 +2818,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2471,16 +2850,16 @@
         <v>11</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>3000</v>
       </c>
       <c r="D2">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>23784</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2488,16 +2867,16 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>680</v>
       </c>
       <c r="D3">
-        <v>5440</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>23784</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2505,16 +2884,16 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>10</v>
       </c>
       <c r="D4">
-        <v>1500</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>23784</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2522,16 +2901,16 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>200</v>
       </c>
       <c r="D5">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>23784</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2539,16 +2918,16 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>129</v>
       </c>
       <c r="D6">
-        <v>129</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>23784</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2556,16 +2935,16 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>145</v>
       </c>
       <c r="D7">
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>23784</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2573,16 +2952,16 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <v>950</v>
       </c>
       <c r="D8">
-        <v>950</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>23784</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2590,16 +2969,16 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9">
         <v>1400</v>
       </c>
       <c r="D9">
-        <v>1400</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>23784</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2607,16 +2986,16 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10">
         <v>1400</v>
       </c>
       <c r="D10">
-        <v>1400</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>23784</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2624,16 +3003,16 @@
         <v>8</v>
       </c>
       <c r="B11">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C11">
         <v>110</v>
       </c>
       <c r="D11">
-        <v>1320</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>23784</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2641,16 +3020,16 @@
         <v>9</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C12">
         <v>500</v>
       </c>
       <c r="D12">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>23784</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2658,16 +3037,16 @@
         <v>10</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C13">
         <v>500</v>
       </c>
       <c r="D13">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>23784</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2675,16 +3054,16 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14">
         <v>900</v>
       </c>
       <c r="D14">
-        <v>900</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>23784</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2692,16 +3071,16 @@
         <v>54</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15">
         <v>400</v>
       </c>
       <c r="D15">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>23784</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2709,16 +3088,16 @@
         <v>13</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16">
         <v>3000</v>
       </c>
       <c r="D16">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>23784</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2726,16 +3105,16 @@
         <v>14</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17">
         <v>1000</v>
       </c>
       <c r="D17">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>23784</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2743,7 +3122,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>

</xml_diff>

<commit_message>
corrected the duplicate entry happening due to cash based transaction
</commit_message>
<xml_diff>
--- a/data/monthly_exp.xlsx
+++ b/data/monthly_exp.xlsx
@@ -9,17 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="734" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="734" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Estimated" sheetId="1" r:id="rId1"/>
     <sheet name="current_total_expense_base" sheetId="8" r:id="rId2"/>
     <sheet name="Actual" sheetId="2" r:id="rId3"/>
-    <sheet name="App_Layout" sheetId="3" r:id="rId4"/>
-    <sheet name="actual_cost_v1" sheetId="4" r:id="rId5"/>
-    <sheet name="current_total_expense_v1" sheetId="5" r:id="rId6"/>
-    <sheet name="planned_estimated_cost_v1" sheetId="7" r:id="rId7"/>
-    <sheet name="expense_growth_rate_v1" sheetId="6" r:id="rId8"/>
+    <sheet name="actual_cost_v1" sheetId="4" r:id="rId4"/>
+    <sheet name="current_total_expense_v1" sheetId="5" r:id="rId5"/>
+    <sheet name="planned_estimated_cost_v1" sheetId="7" r:id="rId6"/>
+    <sheet name="expense_growth_rate_v1" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="46">
   <si>
     <t>rum</t>
   </si>
@@ -157,42 +156,6 @@
   </si>
   <si>
     <t>quantity/Green</t>
-  </si>
-  <si>
-    <t>Webform</t>
-  </si>
-  <si>
-    <t>Commodity Type</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>Radiobutton</t>
-  </si>
-  <si>
-    <t>text box</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Post API Call To Flask Server</t>
-  </si>
-  <si>
-    <t>/submit_data</t>
-  </si>
-  <si>
-    <t>Get API call to /fetch_expense_gr</t>
-  </si>
-  <si>
-    <t>GET API call to fetch account details</t>
-  </si>
-  <si>
-    <t>Cron job for every 6 hours</t>
-  </si>
-  <si>
-    <t>cron job for every 12 hours</t>
   </si>
   <si>
     <t>ParkFee</t>
@@ -634,7 +597,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D16"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F4:F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,7 +883,7 @@
         <v>19</v>
       </c>
       <c r="F1" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1165,7 +1128,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1273,7 +1236,7 @@
   <dimension ref="A1:W24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E18"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1933,7 +1896,7 @@
     </row>
     <row r="14" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2018,7 +1981,7 @@
         <v>31</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
@@ -2054,7 +2017,7 @@
         <v>32</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
@@ -2089,7 +2052,7 @@
         <v>33</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
@@ -2108,7 +2071,7 @@
         <v>33</v>
       </c>
       <c r="N19" s="15" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
@@ -2127,7 +2090,7 @@
         <v>34</v>
       </c>
       <c r="N20" s="15" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
@@ -2146,7 +2109,7 @@
         <v>35</v>
       </c>
       <c r="N21" s="15" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
@@ -2162,10 +2125,10 @@
         <v>10</v>
       </c>
       <c r="M22" s="14" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="N22" s="15" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
@@ -2184,7 +2147,7 @@
         <v>36</v>
       </c>
       <c r="N23" s="15" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
@@ -2222,231 +2185,318 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>3000</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>8774</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>680</v>
+      </c>
+      <c r="D3">
+        <v>2720</v>
+      </c>
+      <c r="E3">
+        <v>7080</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>56</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>560</v>
+      </c>
+      <c r="E4">
+        <v>7080</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>200</v>
+      </c>
+      <c r="D5">
+        <v>200</v>
+      </c>
+      <c r="E5">
+        <v>7080</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>129</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>7080</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>145</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>7080</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>950</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>7080</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>790</v>
+      </c>
+      <c r="D9">
+        <v>790</v>
+      </c>
+      <c r="E9">
+        <v>7080</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1160</v>
+      </c>
+      <c r="D10">
+        <v>1160</v>
+      </c>
+      <c r="E10">
+        <v>7080</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>110</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>7080</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>700</v>
+      </c>
+      <c r="D12">
+        <v>700</v>
+      </c>
+      <c r="E12">
+        <v>7080</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>270</v>
+      </c>
+      <c r="D13">
+        <v>270</v>
+      </c>
+      <c r="E13">
+        <v>7080</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" t="s">
-        <v>50</v>
-      </c>
-      <c r="K8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" t="b">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>680</v>
-      </c>
-      <c r="D9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" t="b">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" t="b">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" t="b">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" t="b">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" t="b">
+      <c r="B14">
         <v>1</v>
       </c>
       <c r="C14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>400</v>
+      </c>
+      <c r="D14">
+        <v>400</v>
+      </c>
+      <c r="E14">
+        <v>7080</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" t="b">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>900</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>7080</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="B16" t="b">
-        <v>0</v>
+      <c r="B16">
+        <v>1</v>
       </c>
       <c r="C16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1849</v>
+      </c>
+      <c r="D16">
+        <v>1849</v>
+      </c>
+      <c r="E16">
+        <v>7080</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
-      <c r="B17" t="b">
+      <c r="B17">
         <v>1</v>
       </c>
       <c r="C17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" t="s">
-        <v>23</v>
-      </c>
-      <c r="G19" t="s">
-        <v>51</v>
-      </c>
-      <c r="K19" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19826</v>
-      </c>
-      <c r="B20">
-        <v>17557</v>
-      </c>
-      <c r="C20">
-        <v>31</v>
-      </c>
-      <c r="D20">
-        <v>3269</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23">
+        <v>125</v>
+      </c>
+      <c r="D17">
+        <v>125</v>
+      </c>
+      <c r="E17">
+        <v>7080</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
         <v>1000</v>
+      </c>
+      <c r="D18">
+        <v>1000</v>
+      </c>
+      <c r="E18">
+        <v>7080</v>
       </c>
     </row>
   </sheetData>
@@ -2456,318 +2506,40 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E18"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>21000</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>11226</v>
       </c>
       <c r="C2">
-        <v>3000</v>
+        <v>24</v>
       </c>
       <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>8774</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>680</v>
-      </c>
-      <c r="D3">
-        <v>2720</v>
-      </c>
-      <c r="E3">
-        <v>7080</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>56</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>560</v>
-      </c>
-      <c r="E4">
-        <v>7080</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>200</v>
-      </c>
-      <c r="D5">
-        <v>200</v>
-      </c>
-      <c r="E5">
-        <v>7080</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>129</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>7080</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>145</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>7080</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>950</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>7080</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>790</v>
-      </c>
-      <c r="D9">
-        <v>790</v>
-      </c>
-      <c r="E9">
-        <v>7080</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>1160</v>
-      </c>
-      <c r="D10">
-        <v>1160</v>
-      </c>
-      <c r="E10">
-        <v>7080</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>110</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>7080</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>700</v>
-      </c>
-      <c r="D12">
-        <v>700</v>
-      </c>
-      <c r="E12">
-        <v>7080</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>270</v>
-      </c>
-      <c r="D13">
-        <v>270</v>
-      </c>
-      <c r="E13">
-        <v>7080</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>400</v>
-      </c>
-      <c r="D14">
-        <v>400</v>
-      </c>
-      <c r="E14">
-        <v>7080</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>900</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>7080</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16">
-        <v>1849</v>
-      </c>
-      <c r="D16">
-        <v>1849</v>
-      </c>
-      <c r="E16">
-        <v>7080</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17">
-        <v>125</v>
-      </c>
-      <c r="D17">
-        <v>125</v>
-      </c>
-      <c r="E17">
-        <v>7080</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
         <v>1000</v>
-      </c>
-      <c r="D18">
-        <v>1000</v>
-      </c>
-      <c r="E18">
-        <v>7080</v>
       </c>
     </row>
   </sheetData>
@@ -2777,52 +2549,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>21000</v>
-      </c>
-      <c r="B2">
-        <v>11226</v>
-      </c>
-      <c r="C2">
-        <v>24</v>
-      </c>
-      <c r="D2">
-        <v>1000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D17"/>
     </sheetView>
   </sheetViews>
@@ -3068,7 +2797,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -3122,7 +2851,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>

</xml_diff>

<commit_message>
added the changes for cash base entry on month end
</commit_message>
<xml_diff>
--- a/data/monthly_exp.xlsx
+++ b/data/monthly_exp.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="734" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="734" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Estimated" sheetId="1" r:id="rId1"/>
@@ -597,7 +597,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,10 +900,10 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>8774</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -911,16 +911,16 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>680</v>
       </c>
       <c r="D3">
-        <v>2720</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>7080</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -931,16 +931,16 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>10</v>
       </c>
       <c r="D4">
-        <v>560</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>7080</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -951,19 +951,19 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>200</v>
       </c>
       <c r="D5">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>7080</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -980,10 +980,10 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>7080</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1000,10 +1000,10 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>7080</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1020,10 +1020,10 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>7080</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1031,19 +1031,19 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9">
         <v>790</v>
       </c>
       <c r="D9">
-        <v>790</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>7080</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1051,19 +1051,19 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10">
         <v>1160</v>
       </c>
       <c r="D10">
-        <v>1160</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>7080</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1080,7 +1080,7 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>7080</v>
+        <v>0</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1091,19 +1091,19 @@
         <v>9</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12">
         <v>700</v>
       </c>
       <c r="D12">
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>7080</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1111,19 +1111,19 @@
         <v>10</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13">
         <v>270</v>
       </c>
       <c r="D13">
-        <v>270</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>7080</v>
+        <v>0</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1131,19 +1131,19 @@
         <v>42</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14">
         <v>400</v>
       </c>
       <c r="D14">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>7080</v>
+        <v>0</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1160,10 +1160,10 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>7080</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1171,19 +1171,19 @@
         <v>13</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16">
         <v>1849</v>
       </c>
       <c r="D16">
-        <v>1849</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>7080</v>
+        <v>0</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1191,19 +1191,19 @@
         <v>14</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17">
         <v>125</v>
       </c>
       <c r="D17">
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>7080</v>
+        <v>0</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1217,13 +1217,13 @@
         <v>1000</v>
       </c>
       <c r="D18">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>7080</v>
+        <v>0</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2508,8 +2508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2533,13 +2533,13 @@
         <v>21000</v>
       </c>
       <c r="B2">
-        <v>11226</v>
+        <v>21000</v>
       </c>
       <c r="C2">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D2">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2552,7 +2552,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D17"/>
+      <selection activeCell="E3" sqref="E3:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2579,16 +2579,17 @@
         <v>11</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>3000</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <f>SUM(D2:D17)</f>
+        <v>23784</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2596,16 +2597,17 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>680</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <f t="shared" ref="D3:D16" si="0">C3*B3</f>
+        <v>5440</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>23784</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2613,16 +2615,17 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="C4">
         <v>10</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1500</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>23784</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2630,16 +2633,17 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>200</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>200</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>23784</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2647,16 +2651,17 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <v>129</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>129</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>23784</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2664,16 +2669,17 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <v>145</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>145</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>23784</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2681,16 +2687,17 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <v>950</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>950</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>23784</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2698,16 +2705,17 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <v>1400</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1400</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>23784</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2715,16 +2723,17 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10">
         <v>1400</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1400</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>23784</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2732,16 +2741,17 @@
         <v>8</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C11">
         <v>110</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1320</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>23784</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2749,16 +2759,17 @@
         <v>9</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C12">
         <v>500</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2000</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>23784</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2766,16 +2777,17 @@
         <v>10</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>500</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1000</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>23784</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2783,16 +2795,17 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <v>900</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>900</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>23784</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2800,16 +2813,17 @@
         <v>42</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15">
         <v>400</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>400</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>23784</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2817,16 +2831,17 @@
         <v>13</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16">
         <v>3000</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3000</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>23784</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2834,16 +2849,16 @@
         <v>14</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17">
         <v>1000</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>23784</v>
       </c>
     </row>
   </sheetData>

</xml_diff>